<commit_message>
modified AI Literacy Lesson Plan
</commit_message>
<xml_diff>
--- a/AI_Literacy_ILT_Materials/Lesson_Plan_AI_Literacy.xlsx
+++ b/AI_Literacy_ILT_Materials/Lesson_Plan_AI_Literacy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29504"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2c4e04267d3dad2/Documents/OutoftheNormAi/Simplilearn/simplilearn-AGS/AI_Literacy_ILT_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{6F28CC9D-6B07-4777-A594-03FB25EB5460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{497177FB-3C06-4CA3-9AE7-E0240749EC0F}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{6F28CC9D-6B07-4777-A594-03FB25EB5460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DD7A367-B995-4A5A-A53B-9C1ABF38BF38}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Class Structure" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -845,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -907,59 +906,62 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1191,12 +1193,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -5638,8 +5640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9F4327-3FAA-42D9-B6A2-ACDDC1A9CD15}">
   <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:G74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76:G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5681,328 +5683,328 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="34">
         <v>1</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="34">
         <v>1</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="4">
         <v>1</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="31">
+      <c r="I2" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41">
+    <row r="3" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
-    </row>
-    <row r="4" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41">
+      <c r="H3" s="31"/>
+      <c r="I3" s="34"/>
+    </row>
+    <row r="4" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="4">
         <v>3</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
-    </row>
-    <row r="5" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41">
+      <c r="H4" s="31"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
-    </row>
-    <row r="6" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41">
+      <c r="H5" s="31"/>
+      <c r="I5" s="34"/>
+    </row>
+    <row r="6" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="4">
         <v>5</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
-    </row>
-    <row r="7" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41">
+      <c r="H6" s="31"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="4">
         <v>6</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-    </row>
-    <row r="8" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41">
+      <c r="H7" s="31"/>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="4">
         <v>7</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
-    </row>
-    <row r="9" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41">
+      <c r="H8" s="31"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="4">
         <v>8</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31"/>
-    </row>
-    <row r="10" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41">
+      <c r="H9" s="31"/>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="4">
         <v>9</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
-    </row>
-    <row r="11" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41">
+      <c r="H10" s="31"/>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="4">
         <v>10</v>
       </c>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
-    </row>
-    <row r="12" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41">
+      <c r="H11" s="31"/>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="4">
         <v>11</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="31"/>
-    </row>
-    <row r="13" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41">
+      <c r="H12" s="31"/>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="4">
         <v>12</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
-    </row>
-    <row r="14" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41">
+      <c r="H13" s="31"/>
+      <c r="I13" s="34"/>
+    </row>
+    <row r="14" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="4">
         <v>13</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31"/>
-    </row>
-    <row r="15" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42" t="s">
+      <c r="H14" s="31"/>
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="31"/>
-    </row>
-    <row r="16" spans="1:9" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="31">
+      <c r="H15" s="31"/>
+      <c r="I15" s="34"/>
+    </row>
+    <row r="16" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="34">
         <v>2</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="4">
         <v>1</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="30"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="4">
         <v>2</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="30"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="4">
         <v>3</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="30"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="4">
         <v>4</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="34"/>
     </row>
     <row r="20" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="30"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="4">
         <v>5</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="34"/>
     </row>
     <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="30"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="4"/>
       <c r="G21" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="34"/>
     </row>
     <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="31">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="34">
         <v>3</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="32" t="s">
         <v>45</v>
       </c>
       <c r="F22" s="4">
@@ -6011,75 +6013,75 @@
       <c r="G22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="29"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="4">
         <v>2</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="34"/>
     </row>
     <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="29"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="4">
         <v>3</v>
       </c>
       <c r="G24" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="34"/>
     </row>
     <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="29"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="4">
         <v>4</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="34"/>
     </row>
     <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="29"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="4"/>
       <c r="G26" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="34"/>
     </row>
     <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="31">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="34">
         <v>4</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="31" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="4">
@@ -6088,99 +6090,99 @@
       <c r="G27" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="30"/>
-      <c r="I27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="34"/>
     </row>
     <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="30"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="4">
         <v>2</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="34"/>
     </row>
     <row r="29" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="30"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="4">
         <v>3</v>
       </c>
       <c r="G29" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="34"/>
     </row>
     <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="30"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="4">
         <v>4</v>
       </c>
       <c r="G30" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="30"/>
-      <c r="I30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="34"/>
     </row>
     <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="30"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="4">
         <v>5</v>
       </c>
       <c r="G31" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="30"/>
-      <c r="I31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="34"/>
     </row>
     <row r="32" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="30"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="31"/>
       <c r="F32" s="4">
         <v>6</v>
       </c>
       <c r="G32" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H32" s="30"/>
-      <c r="I32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="30"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="4"/>
       <c r="G33" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -6191,635 +6193,635 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31">
+      <c r="A35" s="34"/>
+      <c r="B35" s="34">
         <v>2</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="33">
+      <c r="D35" s="40">
         <v>1</v>
       </c>
-      <c r="E35" s="43" t="s">
+      <c r="E35" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F35" s="26">
+      <c r="F35" s="42">
         <v>1</v>
       </c>
-      <c r="G35" s="27" t="s">
+      <c r="G35" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="H35" s="29" t="s">
+      <c r="H35" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="I35" s="31">
+      <c r="I35" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="26">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="42">
         <v>2</v>
       </c>
-      <c r="G36" s="27" t="s">
+      <c r="G36" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="34"/>
     </row>
     <row r="37" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="26">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42">
         <v>3</v>
       </c>
-      <c r="G37" s="27" t="s">
+      <c r="G37" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="H37" s="30"/>
-      <c r="I37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="34"/>
     </row>
     <row r="38" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="26">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="42">
         <v>4</v>
       </c>
-      <c r="G38" s="27" t="s">
+      <c r="G38" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="H38" s="30"/>
-      <c r="I38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="34"/>
     </row>
     <row r="39" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="26">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="42">
         <v>5</v>
       </c>
-      <c r="G39" s="27" t="s">
+      <c r="G39" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H39" s="30"/>
-      <c r="I39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="34"/>
     </row>
     <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="26">
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="42">
         <v>6</v>
       </c>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="34"/>
     </row>
     <row r="41" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="26">
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="42">
         <v>7</v>
       </c>
-      <c r="G41" s="27" t="s">
+      <c r="G41" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="H41" s="30"/>
-      <c r="I41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="34"/>
     </row>
     <row r="42" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="26">
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="42">
         <v>8</v>
       </c>
-      <c r="G42" s="27" t="s">
+      <c r="G42" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="H42" s="30"/>
-      <c r="I42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="34"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="26">
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="42">
         <v>9</v>
       </c>
-      <c r="G43" s="27" t="s">
+      <c r="G43" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="H43" s="30"/>
-      <c r="I43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="34"/>
     </row>
     <row r="44" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="27" t="s">
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H44" s="30"/>
-      <c r="I44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="34"/>
     </row>
     <row r="45" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="33">
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="40">
         <v>2</v>
       </c>
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F45" s="26">
+      <c r="F45" s="42">
         <v>1</v>
       </c>
-      <c r="G45" s="27" t="s">
+      <c r="G45" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="30"/>
-      <c r="I45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="34"/>
     </row>
     <row r="46" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="26">
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="42">
         <v>2</v>
       </c>
-      <c r="G46" s="27" t="s">
+      <c r="G46" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="H46" s="30"/>
-      <c r="I46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="34"/>
     </row>
     <row r="47" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="26">
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="42">
         <v>3</v>
       </c>
-      <c r="G47" s="27" t="s">
+      <c r="G47" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="34"/>
     </row>
     <row r="48" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="27" t="s">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H48" s="30"/>
-      <c r="I48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="34"/>
     </row>
     <row r="49" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="33">
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="40">
         <v>3</v>
       </c>
-      <c r="E49" s="43" t="s">
+      <c r="E49" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="26">
+      <c r="F49" s="42">
         <v>1</v>
       </c>
-      <c r="G49" s="27" t="s">
+      <c r="G49" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="H49" s="30"/>
-      <c r="I49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="34"/>
     </row>
     <row r="50" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="26">
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="42">
         <v>2</v>
       </c>
-      <c r="G50" s="27" t="s">
+      <c r="G50" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H50" s="30"/>
-      <c r="I50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="34"/>
     </row>
     <row r="51" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="26">
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="42">
         <v>3</v>
       </c>
-      <c r="G51" s="27" t="s">
+      <c r="G51" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="H51" s="30"/>
-      <c r="I51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="34"/>
     </row>
     <row r="52" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="31"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="27" t="s">
+      <c r="A52" s="34"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H52" s="30"/>
-      <c r="I52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="34"/>
     </row>
     <row r="53" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="31"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="33">
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="40">
         <v>4</v>
       </c>
-      <c r="E53" s="43" t="s">
+      <c r="E53" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="F53" s="26">
+      <c r="F53" s="42">
         <v>1</v>
       </c>
-      <c r="G53" s="27" t="s">
+      <c r="G53" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="H53" s="30"/>
-      <c r="I53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="34"/>
     </row>
     <row r="54" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="31"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="26">
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="42">
         <v>2</v>
       </c>
-      <c r="G54" s="27" t="s">
+      <c r="G54" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="H54" s="30"/>
-      <c r="I54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="34"/>
     </row>
     <row r="55" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="31"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="26">
+      <c r="A55" s="34"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="42">
         <v>3</v>
       </c>
-      <c r="G55" s="27" t="s">
+      <c r="G55" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="H55" s="30"/>
-      <c r="I55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="34"/>
     </row>
     <row r="56" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="31"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="26">
+      <c r="A56" s="34"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="42">
         <v>4</v>
       </c>
-      <c r="G56" s="27" t="s">
+      <c r="G56" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="H56" s="30"/>
-      <c r="I56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="34"/>
     </row>
     <row r="57" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="31"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="27" t="s">
+      <c r="A57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H57" s="30"/>
-      <c r="I57" s="31"/>
+      <c r="H57" s="31"/>
+      <c r="I57" s="34"/>
     </row>
     <row r="58" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="31"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="33">
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="40">
         <v>5</v>
       </c>
-      <c r="E58" s="43" t="s">
+      <c r="E58" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="F58" s="26">
+      <c r="F58" s="42">
         <v>1</v>
       </c>
-      <c r="G58" s="27" t="s">
+      <c r="G58" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="H58" s="30"/>
-      <c r="I58" s="31"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="34"/>
     </row>
     <row r="59" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="26">
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="42">
         <v>2</v>
       </c>
-      <c r="G59" s="27" t="s">
+      <c r="G59" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="H59" s="30"/>
-      <c r="I59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="34"/>
     </row>
     <row r="60" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="31"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="26">
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="42">
         <v>3</v>
       </c>
-      <c r="G60" s="27" t="s">
+      <c r="G60" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="H60" s="30"/>
-      <c r="I60" s="31"/>
+      <c r="H60" s="31"/>
+      <c r="I60" s="34"/>
     </row>
     <row r="61" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="31"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="26">
+      <c r="A61" s="34"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="42">
         <v>4</v>
       </c>
-      <c r="G61" s="27" t="s">
+      <c r="G61" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="H61" s="30"/>
-      <c r="I61" s="31"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="34"/>
     </row>
     <row r="62" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="31"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="26">
+      <c r="A62" s="34"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="42">
         <v>5</v>
       </c>
-      <c r="G62" s="27" t="s">
+      <c r="G62" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="H62" s="30"/>
-      <c r="I62" s="31"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="34"/>
     </row>
     <row r="63" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="31"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="27" t="s">
+      <c r="A63" s="34"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H63" s="30"/>
-      <c r="I63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="34"/>
     </row>
     <row r="64" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="31"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="33">
+      <c r="A64" s="34"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="40">
         <v>6</v>
       </c>
       <c r="E64" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="F64" s="26">
+      <c r="F64" s="42">
         <v>1</v>
       </c>
-      <c r="G64" s="27" t="s">
+      <c r="G64" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="H64" s="30"/>
-      <c r="I64" s="31"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="34"/>
     </row>
     <row r="65" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="31"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="33"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="40"/>
       <c r="E65" s="44"/>
-      <c r="F65" s="26">
+      <c r="F65" s="42">
         <v>2</v>
       </c>
-      <c r="G65" s="27" t="s">
+      <c r="G65" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="H65" s="30"/>
-      <c r="I65" s="31"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="34"/>
     </row>
     <row r="66" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="31"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="33"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="40"/>
       <c r="E66" s="44"/>
-      <c r="F66" s="26">
+      <c r="F66" s="42">
         <v>3</v>
       </c>
-      <c r="G66" s="27" t="s">
+      <c r="G66" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="H66" s="30"/>
-      <c r="I66" s="31"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="34"/>
     </row>
     <row r="67" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="31"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="33"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="40"/>
       <c r="E67" s="44"/>
-      <c r="F67" s="26">
+      <c r="F67" s="42">
         <v>4</v>
       </c>
-      <c r="G67" s="27" t="s">
+      <c r="G67" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="H67" s="30"/>
-      <c r="I67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="34"/>
     </row>
     <row r="68" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A68" s="31"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="33"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="40"/>
       <c r="E68" s="44"/>
-      <c r="F68" s="26"/>
-      <c r="G68" s="27" t="s">
+      <c r="F68" s="42"/>
+      <c r="G68" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H68" s="30"/>
-      <c r="I68" s="31"/>
+      <c r="H68" s="31"/>
+      <c r="I68" s="34"/>
     </row>
     <row r="69" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A69" s="31"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="29"/>
-      <c r="D69" s="33">
+      <c r="A69" s="34"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="40">
         <v>7</v>
       </c>
-      <c r="E69" s="43" t="s">
+      <c r="E69" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="F69" s="26">
+      <c r="F69" s="42">
         <v>1</v>
       </c>
-      <c r="G69" s="27" t="s">
+      <c r="G69" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="H69" s="30"/>
-      <c r="I69" s="31"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="34"/>
     </row>
     <row r="70" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="31"/>
-      <c r="B70" s="31"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="26">
+      <c r="A70" s="34"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="40"/>
+      <c r="E70" s="41"/>
+      <c r="F70" s="42">
         <v>2</v>
       </c>
-      <c r="G70" s="27" t="s">
+      <c r="G70" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="H70" s="30"/>
-      <c r="I70" s="31"/>
+      <c r="H70" s="31"/>
+      <c r="I70" s="34"/>
     </row>
     <row r="71" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="31"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="27" t="s">
+      <c r="A71" s="34"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="41"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H71" s="30"/>
-      <c r="I71" s="31"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="34"/>
     </row>
     <row r="72" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="31"/>
-      <c r="B72" s="31"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="25">
+      <c r="A72" s="34"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="45">
         <v>8</v>
       </c>
-      <c r="E72" s="45" t="s">
+      <c r="E72" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="F72" s="26">
+      <c r="F72" s="42">
         <v>1</v>
       </c>
-      <c r="G72" s="27" t="s">
+      <c r="G72" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="H72" s="30"/>
-      <c r="I72" s="31"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="34"/>
     </row>
     <row r="73" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A73" s="31"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="33">
+      <c r="A73" s="34"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="40">
         <v>9</v>
       </c>
-      <c r="E73" s="45" t="s">
+      <c r="E73" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="F73" s="26">
+      <c r="F73" s="42">
         <v>1</v>
       </c>
-      <c r="G73" s="27" t="s">
+      <c r="G73" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="H73" s="30"/>
-      <c r="I73" s="31"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="34"/>
     </row>
     <row r="74" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A74" s="31"/>
-      <c r="B74" s="31"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="27" t="s">
+      <c r="A74" s="34"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H74" s="30"/>
-      <c r="I74" s="31"/>
+      <c r="H74" s="31"/>
+      <c r="I74" s="34"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="31"/>
+      <c r="A75" s="34"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -6830,537 +6832,537 @@
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A76" s="31"/>
-      <c r="B76" s="31">
+      <c r="A76" s="34"/>
+      <c r="B76" s="34">
         <v>3</v>
       </c>
-      <c r="C76" s="29" t="s">
+      <c r="C76" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D76" s="31">
+      <c r="D76" s="35">
         <v>1</v>
       </c>
-      <c r="E76" s="30" t="s">
+      <c r="E76" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="F76" s="4">
+      <c r="F76" s="25">
         <v>1</v>
       </c>
-      <c r="G76" s="22" t="s">
+      <c r="G76" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="H76" s="29" t="s">
+      <c r="H76" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="I76" s="31">
+      <c r="I76" s="34">
         <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A77" s="31"/>
-      <c r="B77" s="31"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="4">
+      <c r="A77" s="34"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="25">
         <v>2</v>
       </c>
-      <c r="G77" s="22" t="s">
+      <c r="G77" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="H77" s="30"/>
-      <c r="I77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="34"/>
     </row>
     <row r="78" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="31"/>
-      <c r="B78" s="31"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="4">
+      <c r="A78" s="34"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="25">
         <v>3</v>
       </c>
-      <c r="G78" s="22" t="s">
+      <c r="G78" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="H78" s="30"/>
-      <c r="I78" s="31"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="34"/>
     </row>
     <row r="79" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A79" s="31"/>
-      <c r="B79" s="31"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="4">
+      <c r="A79" s="34"/>
+      <c r="B79" s="34"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="25">
         <v>4</v>
       </c>
-      <c r="G79" s="22" t="s">
+      <c r="G79" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="H79" s="30"/>
-      <c r="I79" s="31"/>
+      <c r="H79" s="31"/>
+      <c r="I79" s="34"/>
     </row>
     <row r="80" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="31"/>
-      <c r="B80" s="31"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="4">
+      <c r="A80" s="34"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="25">
         <v>5</v>
       </c>
-      <c r="G80" s="22" t="s">
+      <c r="G80" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="H80" s="30"/>
-      <c r="I80" s="31"/>
+      <c r="H80" s="31"/>
+      <c r="I80" s="34"/>
     </row>
     <row r="81" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="31"/>
-      <c r="B81" s="31"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="4">
+      <c r="A81" s="34"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="25">
         <v>6</v>
       </c>
-      <c r="G81" s="22" t="s">
+      <c r="G81" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="H81" s="30"/>
-      <c r="I81" s="31"/>
+      <c r="H81" s="31"/>
+      <c r="I81" s="34"/>
     </row>
     <row r="82" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A82" s="31"/>
-      <c r="B82" s="31"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="31"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="22" t="s">
+      <c r="A82" s="34"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H82" s="30"/>
-      <c r="I82" s="31"/>
+      <c r="H82" s="31"/>
+      <c r="I82" s="34"/>
     </row>
     <row r="83" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A83" s="31"/>
-      <c r="B83" s="31"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="31">
+      <c r="A83" s="34"/>
+      <c r="B83" s="34"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="35">
         <v>2</v>
       </c>
-      <c r="E83" s="29" t="s">
+      <c r="E83" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="F83" s="4">
+      <c r="F83" s="25">
         <v>1</v>
       </c>
-      <c r="G83" s="22" t="s">
+      <c r="G83" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="H83" s="30"/>
-      <c r="I83" s="31"/>
+      <c r="H83" s="31"/>
+      <c r="I83" s="34"/>
     </row>
     <row r="84" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A84" s="31"/>
-      <c r="B84" s="31"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="31"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="4">
+      <c r="A84" s="34"/>
+      <c r="B84" s="34"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="25">
         <v>2</v>
       </c>
-      <c r="G84" s="22" t="s">
+      <c r="G84" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H84" s="30"/>
-      <c r="I84" s="31"/>
+      <c r="H84" s="31"/>
+      <c r="I84" s="34"/>
     </row>
     <row r="85" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A85" s="31"/>
-      <c r="B85" s="31"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="22" t="s">
+      <c r="A85" s="34"/>
+      <c r="B85" s="34"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="35"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="30"/>
-      <c r="I85" s="31"/>
+      <c r="H85" s="31"/>
+      <c r="I85" s="34"/>
     </row>
     <row r="86" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A86" s="31"/>
-      <c r="B86" s="31"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="31">
+      <c r="A86" s="34"/>
+      <c r="B86" s="34"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="35">
         <v>3</v>
       </c>
-      <c r="E86" s="29" t="s">
+      <c r="E86" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="F86" s="4">
+      <c r="F86" s="25">
         <v>1</v>
       </c>
-      <c r="G86" s="22" t="s">
+      <c r="G86" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="H86" s="30"/>
-      <c r="I86" s="31"/>
+      <c r="H86" s="31"/>
+      <c r="I86" s="34"/>
     </row>
     <row r="87" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A87" s="31"/>
-      <c r="B87" s="31"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="31"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="4">
+      <c r="A87" s="34"/>
+      <c r="B87" s="34"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="35"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="25">
         <v>2</v>
       </c>
-      <c r="G87" s="22" t="s">
+      <c r="G87" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="H87" s="30"/>
-      <c r="I87" s="31"/>
+      <c r="H87" s="31"/>
+      <c r="I87" s="34"/>
     </row>
     <row r="88" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A88" s="31"/>
-      <c r="B88" s="31"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="31"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="4">
+      <c r="A88" s="34"/>
+      <c r="B88" s="34"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="35"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="25">
         <v>3</v>
       </c>
-      <c r="G88" s="22" t="s">
+      <c r="G88" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="H88" s="30"/>
-      <c r="I88" s="31"/>
+      <c r="H88" s="31"/>
+      <c r="I88" s="34"/>
     </row>
     <row r="89" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A89" s="31"/>
-      <c r="B89" s="31"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="31"/>
-      <c r="E89" s="29"/>
-      <c r="F89" s="4">
+      <c r="A89" s="34"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="35"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="25">
         <v>4</v>
       </c>
-      <c r="G89" s="22" t="s">
+      <c r="G89" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="H89" s="30"/>
-      <c r="I89" s="31"/>
+      <c r="H89" s="31"/>
+      <c r="I89" s="34"/>
     </row>
     <row r="90" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="31"/>
-      <c r="B90" s="31"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="31"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="22" t="s">
+      <c r="A90" s="34"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="35"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H90" s="30"/>
-      <c r="I90" s="31"/>
+      <c r="H90" s="31"/>
+      <c r="I90" s="34"/>
     </row>
     <row r="91" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A91" s="31"/>
-      <c r="B91" s="31"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="29"/>
-      <c r="F91" s="4">
+      <c r="A91" s="34"/>
+      <c r="B91" s="34"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="33"/>
+      <c r="F91" s="25">
         <v>5</v>
       </c>
-      <c r="G91" s="22" t="s">
+      <c r="G91" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="H91" s="30"/>
-      <c r="I91" s="31"/>
+      <c r="H91" s="31"/>
+      <c r="I91" s="34"/>
     </row>
     <row r="92" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A92" s="31"/>
-      <c r="B92" s="31"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="31">
+      <c r="A92" s="34"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="35">
         <v>4</v>
       </c>
-      <c r="E92" s="29" t="s">
+      <c r="E92" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="F92" s="4">
+      <c r="F92" s="25">
         <v>1</v>
       </c>
-      <c r="G92" s="22" t="s">
+      <c r="G92" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="H92" s="30"/>
-      <c r="I92" s="31"/>
+      <c r="H92" s="31"/>
+      <c r="I92" s="34"/>
     </row>
     <row r="93" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="31"/>
-      <c r="B93" s="31"/>
-      <c r="C93" s="29"/>
-      <c r="D93" s="31"/>
-      <c r="E93" s="29"/>
-      <c r="F93" s="4">
+      <c r="A93" s="34"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="33"/>
+      <c r="F93" s="25">
         <v>2</v>
       </c>
-      <c r="G93" s="22" t="s">
+      <c r="G93" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="H93" s="30"/>
-      <c r="I93" s="31"/>
+      <c r="H93" s="31"/>
+      <c r="I93" s="34"/>
     </row>
     <row r="94" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A94" s="31"/>
-      <c r="B94" s="31"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="31"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="22" t="s">
+      <c r="A94" s="34"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="35"/>
+      <c r="E94" s="33"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H94" s="30"/>
-      <c r="I94" s="31"/>
+      <c r="H94" s="31"/>
+      <c r="I94" s="34"/>
     </row>
     <row r="95" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A95" s="31"/>
-      <c r="B95" s="31"/>
-      <c r="C95" s="29"/>
-      <c r="D95" s="31">
+      <c r="A95" s="34"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="35">
         <v>5</v>
       </c>
-      <c r="E95" s="29" t="s">
+      <c r="E95" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="F95" s="4">
+      <c r="F95" s="25">
         <v>1</v>
       </c>
-      <c r="G95" s="22" t="s">
+      <c r="G95" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="H95" s="30"/>
-      <c r="I95" s="31"/>
+      <c r="H95" s="31"/>
+      <c r="I95" s="34"/>
     </row>
     <row r="96" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A96" s="31"/>
-      <c r="B96" s="31"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="31"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="4">
+      <c r="A96" s="34"/>
+      <c r="B96" s="34"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="35"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="25">
         <v>2</v>
       </c>
-      <c r="G96" s="22" t="s">
+      <c r="G96" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="H96" s="30"/>
-      <c r="I96" s="31"/>
+      <c r="H96" s="31"/>
+      <c r="I96" s="34"/>
     </row>
     <row r="97" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A97" s="31"/>
-      <c r="B97" s="31"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="31"/>
-      <c r="E97" s="29"/>
-      <c r="F97" s="4">
+      <c r="A97" s="34"/>
+      <c r="B97" s="34"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="33"/>
+      <c r="F97" s="25">
         <v>3</v>
       </c>
-      <c r="G97" s="22" t="s">
+      <c r="G97" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="H97" s="30"/>
-      <c r="I97" s="31"/>
+      <c r="H97" s="31"/>
+      <c r="I97" s="34"/>
     </row>
     <row r="98" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A98" s="31"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="31"/>
-      <c r="E98" s="29"/>
-      <c r="F98" s="4">
+      <c r="A98" s="34"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="25">
         <v>4</v>
       </c>
-      <c r="G98" s="22" t="s">
+      <c r="G98" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="H98" s="30"/>
-      <c r="I98" s="31"/>
+      <c r="H98" s="31"/>
+      <c r="I98" s="34"/>
     </row>
     <row r="99" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A99" s="31"/>
-      <c r="B99" s="31"/>
-      <c r="C99" s="29"/>
-      <c r="D99" s="31"/>
-      <c r="E99" s="29"/>
-      <c r="F99" s="4">
+      <c r="A99" s="34"/>
+      <c r="B99" s="34"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="33"/>
+      <c r="F99" s="25">
         <v>5</v>
       </c>
-      <c r="G99" s="22" t="s">
+      <c r="G99" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="H99" s="30"/>
-      <c r="I99" s="31"/>
+      <c r="H99" s="31"/>
+      <c r="I99" s="34"/>
     </row>
     <row r="100" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A100" s="31"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="29"/>
-      <c r="D100" s="31"/>
-      <c r="E100" s="29"/>
-      <c r="F100" s="4">
+      <c r="A100" s="34"/>
+      <c r="B100" s="34"/>
+      <c r="C100" s="32"/>
+      <c r="D100" s="35"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="25">
         <v>6</v>
       </c>
-      <c r="G100" s="22" t="s">
+      <c r="G100" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="H100" s="30"/>
-      <c r="I100" s="31"/>
+      <c r="H100" s="31"/>
+      <c r="I100" s="34"/>
     </row>
     <row r="101" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="31"/>
-      <c r="B101" s="31"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="31"/>
-      <c r="E101" s="29"/>
-      <c r="F101" s="4">
+      <c r="A101" s="34"/>
+      <c r="B101" s="34"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="33"/>
+      <c r="F101" s="25">
         <v>7</v>
       </c>
-      <c r="G101" s="22" t="s">
+      <c r="G101" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="H101" s="30"/>
-      <c r="I101" s="31"/>
+      <c r="H101" s="31"/>
+      <c r="I101" s="34"/>
     </row>
     <row r="102" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A102" s="31"/>
-      <c r="B102" s="31"/>
-      <c r="C102" s="29"/>
-      <c r="D102" s="31"/>
-      <c r="E102" s="29"/>
-      <c r="F102" s="4">
+      <c r="A102" s="34"/>
+      <c r="B102" s="34"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="35"/>
+      <c r="E102" s="33"/>
+      <c r="F102" s="25">
         <v>8</v>
       </c>
-      <c r="G102" s="22" t="s">
+      <c r="G102" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="H102" s="30"/>
-      <c r="I102" s="31"/>
+      <c r="H102" s="31"/>
+      <c r="I102" s="34"/>
     </row>
     <row r="103" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A103" s="31"/>
-      <c r="B103" s="31"/>
-      <c r="C103" s="29"/>
-      <c r="D103" s="31"/>
-      <c r="E103" s="29"/>
-      <c r="F103" s="4">
+      <c r="A103" s="34"/>
+      <c r="B103" s="34"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="33"/>
+      <c r="F103" s="25">
         <v>9</v>
       </c>
-      <c r="G103" s="22" t="s">
+      <c r="G103" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="H103" s="30"/>
-      <c r="I103" s="31"/>
+      <c r="H103" s="31"/>
+      <c r="I103" s="34"/>
     </row>
     <row r="104" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A104" s="31"/>
-      <c r="B104" s="31"/>
-      <c r="C104" s="29"/>
-      <c r="D104" s="31"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="22" t="s">
+      <c r="A104" s="34"/>
+      <c r="B104" s="34"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="35"/>
+      <c r="E104" s="33"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H104" s="30"/>
-      <c r="I104" s="31"/>
+      <c r="H104" s="31"/>
+      <c r="I104" s="34"/>
     </row>
     <row r="105" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A105" s="31"/>
-      <c r="B105" s="31"/>
-      <c r="C105" s="29"/>
-      <c r="D105" s="31">
+      <c r="A105" s="34"/>
+      <c r="B105" s="34"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="35">
         <v>6</v>
       </c>
-      <c r="E105" s="29" t="s">
+      <c r="E105" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="F105" s="4">
+      <c r="F105" s="25">
         <v>1</v>
       </c>
-      <c r="G105" s="22" t="s">
+      <c r="G105" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="H105" s="30"/>
-      <c r="I105" s="31"/>
+      <c r="H105" s="31"/>
+      <c r="I105" s="34"/>
     </row>
     <row r="106" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A106" s="31"/>
-      <c r="B106" s="31"/>
-      <c r="C106" s="29"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="29"/>
-      <c r="F106" s="4">
+      <c r="A106" s="34"/>
+      <c r="B106" s="34"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="35"/>
+      <c r="E106" s="33"/>
+      <c r="F106" s="25">
         <v>2</v>
       </c>
-      <c r="G106" s="22" t="s">
+      <c r="G106" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="H106" s="30"/>
-      <c r="I106" s="31"/>
+      <c r="H106" s="31"/>
+      <c r="I106" s="34"/>
     </row>
     <row r="107" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A107" s="31"/>
-      <c r="B107" s="31"/>
-      <c r="C107" s="29"/>
-      <c r="D107" s="31"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="4">
+      <c r="A107" s="34"/>
+      <c r="B107" s="34"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="33"/>
+      <c r="F107" s="25">
         <v>3</v>
       </c>
-      <c r="G107" s="22" t="s">
+      <c r="G107" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H107" s="30"/>
-      <c r="I107" s="31"/>
+      <c r="H107" s="31"/>
+      <c r="I107" s="34"/>
     </row>
     <row r="108" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A108" s="31"/>
-      <c r="B108" s="31"/>
-      <c r="C108" s="29"/>
-      <c r="D108" s="31"/>
-      <c r="E108" s="29"/>
-      <c r="F108" s="4"/>
-      <c r="G108" s="22" t="s">
+      <c r="A108" s="34"/>
+      <c r="B108" s="34"/>
+      <c r="C108" s="32"/>
+      <c r="D108" s="35"/>
+      <c r="E108" s="33"/>
+      <c r="F108" s="25"/>
+      <c r="G108" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H108" s="30"/>
-      <c r="I108" s="31"/>
+      <c r="H108" s="31"/>
+      <c r="I108" s="34"/>
     </row>
     <row r="109" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A109" s="31"/>
-      <c r="B109" s="31"/>
-      <c r="C109" s="29"/>
-      <c r="D109" s="31"/>
-      <c r="E109" s="29"/>
-      <c r="F109" s="4">
+      <c r="A109" s="34"/>
+      <c r="B109" s="34"/>
+      <c r="C109" s="32"/>
+      <c r="D109" s="35"/>
+      <c r="E109" s="33"/>
+      <c r="F109" s="25">
         <v>4</v>
       </c>
-      <c r="G109" s="22" t="s">
+      <c r="G109" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H109" s="30"/>
-      <c r="I109" s="31"/>
+      <c r="H109" s="31"/>
+      <c r="I109" s="34"/>
     </row>
     <row r="110" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A110" s="31"/>
+      <c r="A110" s="34"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
@@ -7371,17 +7373,17 @@
       <c r="I110" s="4"/>
     </row>
     <row r="111" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A111" s="31"/>
-      <c r="B111" s="31">
+      <c r="A111" s="34"/>
+      <c r="B111" s="34">
         <v>4</v>
       </c>
-      <c r="C111" s="29" t="s">
+      <c r="C111" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="D111" s="31">
+      <c r="D111" s="34">
         <v>1</v>
       </c>
-      <c r="E111" s="29" t="s">
+      <c r="E111" s="32" t="s">
         <v>132</v>
       </c>
       <c r="F111" s="4">
@@ -7390,66 +7392,66 @@
       <c r="G111" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="H111" s="29" t="s">
+      <c r="H111" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="I111" s="31">
+      <c r="I111" s="34">
         <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A112" s="31"/>
-      <c r="B112" s="31"/>
-      <c r="C112" s="29"/>
-      <c r="D112" s="31"/>
-      <c r="E112" s="29"/>
+      <c r="A112" s="34"/>
+      <c r="B112" s="34"/>
+      <c r="C112" s="32"/>
+      <c r="D112" s="34"/>
+      <c r="E112" s="32"/>
       <c r="F112" s="4">
         <v>2</v>
       </c>
       <c r="G112" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="H112" s="30"/>
-      <c r="I112" s="31"/>
+      <c r="H112" s="31"/>
+      <c r="I112" s="34"/>
     </row>
     <row r="113" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="31"/>
-      <c r="B113" s="31"/>
-      <c r="C113" s="29"/>
-      <c r="D113" s="31"/>
-      <c r="E113" s="29"/>
+      <c r="A113" s="34"/>
+      <c r="B113" s="34"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="34"/>
+      <c r="E113" s="32"/>
       <c r="F113" s="4">
         <v>3</v>
       </c>
       <c r="G113" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="H113" s="30"/>
-      <c r="I113" s="31"/>
+      <c r="H113" s="31"/>
+      <c r="I113" s="34"/>
     </row>
     <row r="114" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="31"/>
-      <c r="B114" s="31"/>
-      <c r="C114" s="29"/>
-      <c r="D114" s="31"/>
-      <c r="E114" s="29"/>
+      <c r="A114" s="34"/>
+      <c r="B114" s="34"/>
+      <c r="C114" s="32"/>
+      <c r="D114" s="34"/>
+      <c r="E114" s="32"/>
       <c r="F114" s="4">
         <v>4</v>
       </c>
       <c r="G114" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="H114" s="30"/>
-      <c r="I114" s="31"/>
+      <c r="H114" s="31"/>
+      <c r="I114" s="34"/>
     </row>
     <row r="115" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A115" s="31"/>
-      <c r="B115" s="31"/>
-      <c r="C115" s="29"/>
-      <c r="D115" s="31">
+      <c r="A115" s="34"/>
+      <c r="B115" s="34"/>
+      <c r="C115" s="32"/>
+      <c r="D115" s="34">
         <v>2</v>
       </c>
-      <c r="E115" s="29" t="s">
+      <c r="E115" s="32" t="s">
         <v>138</v>
       </c>
       <c r="F115" s="4">
@@ -7458,47 +7460,47 @@
       <c r="G115" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="H115" s="30"/>
-      <c r="I115" s="31"/>
+      <c r="H115" s="31"/>
+      <c r="I115" s="34"/>
     </row>
     <row r="116" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="31"/>
-      <c r="B116" s="31"/>
-      <c r="C116" s="29"/>
-      <c r="D116" s="31"/>
-      <c r="E116" s="29"/>
+      <c r="A116" s="34"/>
+      <c r="B116" s="34"/>
+      <c r="C116" s="32"/>
+      <c r="D116" s="34"/>
+      <c r="E116" s="32"/>
       <c r="F116" s="4">
         <v>2</v>
       </c>
       <c r="G116" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="H116" s="30"/>
-      <c r="I116" s="31"/>
+      <c r="H116" s="31"/>
+      <c r="I116" s="34"/>
     </row>
     <row r="117" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A117" s="31"/>
-      <c r="B117" s="31"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="31"/>
-      <c r="E117" s="29"/>
+      <c r="A117" s="34"/>
+      <c r="B117" s="34"/>
+      <c r="C117" s="32"/>
+      <c r="D117" s="34"/>
+      <c r="E117" s="32"/>
       <c r="F117" s="4">
         <v>3</v>
       </c>
       <c r="G117" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="H117" s="30"/>
-      <c r="I117" s="31"/>
+      <c r="H117" s="31"/>
+      <c r="I117" s="34"/>
     </row>
     <row r="118" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A118" s="31"/>
-      <c r="B118" s="31"/>
-      <c r="C118" s="29"/>
-      <c r="D118" s="31">
+      <c r="A118" s="34"/>
+      <c r="B118" s="34"/>
+      <c r="C118" s="32"/>
+      <c r="D118" s="34">
         <v>3</v>
       </c>
-      <c r="E118" s="29" t="s">
+      <c r="E118" s="32" t="s">
         <v>141</v>
       </c>
       <c r="F118" s="4">
@@ -7507,212 +7509,212 @@
       <c r="G118" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="H118" s="30"/>
-      <c r="I118" s="31"/>
+      <c r="H118" s="31"/>
+      <c r="I118" s="34"/>
     </row>
     <row r="119" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A119" s="31"/>
-      <c r="B119" s="31"/>
-      <c r="C119" s="29"/>
-      <c r="D119" s="31"/>
-      <c r="E119" s="29"/>
+      <c r="A119" s="34"/>
+      <c r="B119" s="34"/>
+      <c r="C119" s="32"/>
+      <c r="D119" s="34"/>
+      <c r="E119" s="32"/>
       <c r="F119" s="4">
         <v>2</v>
       </c>
       <c r="G119" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="H119" s="30"/>
-      <c r="I119" s="31"/>
+      <c r="H119" s="31"/>
+      <c r="I119" s="34"/>
     </row>
     <row r="120" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A120" s="31"/>
-      <c r="B120" s="31"/>
-      <c r="C120" s="29"/>
-      <c r="D120" s="31"/>
-      <c r="E120" s="29"/>
+      <c r="A120" s="34"/>
+      <c r="B120" s="34"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="34"/>
+      <c r="E120" s="32"/>
       <c r="F120" s="4">
         <v>3</v>
       </c>
       <c r="G120" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="H120" s="30"/>
-      <c r="I120" s="31"/>
+      <c r="H120" s="31"/>
+      <c r="I120" s="34"/>
     </row>
     <row r="121" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A121" s="31"/>
-      <c r="B121" s="31"/>
-      <c r="C121" s="29"/>
-      <c r="D121" s="31"/>
-      <c r="E121" s="29"/>
+      <c r="A121" s="34"/>
+      <c r="B121" s="34"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="34"/>
+      <c r="E121" s="32"/>
       <c r="F121" s="4">
         <v>4</v>
       </c>
       <c r="G121" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="H121" s="30"/>
-      <c r="I121" s="31"/>
+      <c r="H121" s="31"/>
+      <c r="I121" s="34"/>
     </row>
     <row r="122" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A122" s="31"/>
-      <c r="B122" s="31"/>
-      <c r="C122" s="29"/>
-      <c r="D122" s="31"/>
-      <c r="E122" s="29"/>
+      <c r="A122" s="34"/>
+      <c r="B122" s="34"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="34"/>
+      <c r="E122" s="32"/>
       <c r="F122" s="4">
         <v>5</v>
       </c>
       <c r="G122" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="H122" s="30"/>
-      <c r="I122" s="31"/>
+      <c r="H122" s="31"/>
+      <c r="I122" s="34"/>
     </row>
     <row r="123" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A123" s="31"/>
-      <c r="B123" s="31"/>
-      <c r="C123" s="29"/>
-      <c r="D123" s="31"/>
-      <c r="E123" s="29"/>
+      <c r="A123" s="34"/>
+      <c r="B123" s="34"/>
+      <c r="C123" s="32"/>
+      <c r="D123" s="34"/>
+      <c r="E123" s="32"/>
       <c r="F123" s="4">
         <v>6</v>
       </c>
       <c r="G123" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="H123" s="30"/>
-      <c r="I123" s="31"/>
+      <c r="H123" s="31"/>
+      <c r="I123" s="34"/>
     </row>
     <row r="124" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A124" s="31"/>
-      <c r="B124" s="31"/>
-      <c r="C124" s="29"/>
-      <c r="D124" s="31"/>
-      <c r="E124" s="29"/>
+      <c r="A124" s="34"/>
+      <c r="B124" s="34"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="34"/>
+      <c r="E124" s="32"/>
       <c r="F124" s="4">
         <v>7</v>
       </c>
       <c r="G124" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="H124" s="30"/>
-      <c r="I124" s="31"/>
+      <c r="H124" s="31"/>
+      <c r="I124" s="34"/>
     </row>
     <row r="125" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A125" s="31"/>
-      <c r="B125" s="31"/>
-      <c r="C125" s="29"/>
-      <c r="D125" s="31"/>
-      <c r="E125" s="29"/>
+      <c r="A125" s="34"/>
+      <c r="B125" s="34"/>
+      <c r="C125" s="32"/>
+      <c r="D125" s="34"/>
+      <c r="E125" s="32"/>
       <c r="F125" s="4">
         <v>8</v>
       </c>
       <c r="G125" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="H125" s="30"/>
-      <c r="I125" s="31"/>
+      <c r="H125" s="31"/>
+      <c r="I125" s="34"/>
     </row>
     <row r="126" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A126" s="31"/>
-      <c r="B126" s="31"/>
-      <c r="C126" s="29"/>
-      <c r="D126" s="31"/>
-      <c r="E126" s="29"/>
+      <c r="A126" s="34"/>
+      <c r="B126" s="34"/>
+      <c r="C126" s="32"/>
+      <c r="D126" s="34"/>
+      <c r="E126" s="32"/>
       <c r="F126" s="4">
         <v>9</v>
       </c>
       <c r="G126" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="H126" s="30"/>
-      <c r="I126" s="31"/>
+      <c r="H126" s="31"/>
+      <c r="I126" s="34"/>
     </row>
     <row r="127" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A127" s="31"/>
-      <c r="B127" s="31"/>
-      <c r="C127" s="29"/>
-      <c r="D127" s="31"/>
-      <c r="E127" s="29"/>
+      <c r="A127" s="34"/>
+      <c r="B127" s="34"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="34"/>
+      <c r="E127" s="32"/>
       <c r="F127" s="4">
         <v>10</v>
       </c>
       <c r="G127" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="H127" s="30"/>
-      <c r="I127" s="31"/>
+      <c r="H127" s="31"/>
+      <c r="I127" s="34"/>
     </row>
     <row r="128" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A128" s="31"/>
-      <c r="B128" s="31"/>
-      <c r="C128" s="29"/>
-      <c r="D128" s="31"/>
-      <c r="E128" s="29"/>
+      <c r="A128" s="34"/>
+      <c r="B128" s="34"/>
+      <c r="C128" s="32"/>
+      <c r="D128" s="34"/>
+      <c r="E128" s="32"/>
       <c r="F128" s="4">
         <v>11</v>
       </c>
       <c r="G128" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="H128" s="30"/>
-      <c r="I128" s="31"/>
+      <c r="H128" s="31"/>
+      <c r="I128" s="34"/>
     </row>
     <row r="129" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A129" s="31"/>
-      <c r="B129" s="31"/>
-      <c r="C129" s="29"/>
-      <c r="D129" s="31"/>
-      <c r="E129" s="29"/>
+      <c r="A129" s="34"/>
+      <c r="B129" s="34"/>
+      <c r="C129" s="32"/>
+      <c r="D129" s="34"/>
+      <c r="E129" s="32"/>
       <c r="F129" s="4">
         <v>12</v>
       </c>
       <c r="G129" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="H129" s="30"/>
-      <c r="I129" s="31"/>
+      <c r="H129" s="31"/>
+      <c r="I129" s="34"/>
     </row>
     <row r="130" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A130" s="31"/>
-      <c r="B130" s="31"/>
-      <c r="C130" s="29"/>
-      <c r="D130" s="31"/>
-      <c r="E130" s="29"/>
+      <c r="A130" s="34"/>
+      <c r="B130" s="34"/>
+      <c r="C130" s="32"/>
+      <c r="D130" s="34"/>
+      <c r="E130" s="32"/>
       <c r="F130" s="4">
         <v>13</v>
       </c>
       <c r="G130" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="H130" s="30"/>
-      <c r="I130" s="31"/>
+      <c r="H130" s="31"/>
+      <c r="I130" s="34"/>
     </row>
     <row r="131" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A131" s="31"/>
-      <c r="B131" s="31"/>
-      <c r="C131" s="29"/>
-      <c r="D131" s="31"/>
-      <c r="E131" s="29"/>
+      <c r="A131" s="34"/>
+      <c r="B131" s="34"/>
+      <c r="C131" s="32"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="32"/>
       <c r="F131" s="4">
         <v>14</v>
       </c>
       <c r="G131" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="H131" s="30"/>
-      <c r="I131" s="31"/>
+      <c r="H131" s="31"/>
+      <c r="I131" s="34"/>
     </row>
     <row r="132" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A132" s="31"/>
-      <c r="B132" s="31"/>
-      <c r="C132" s="29"/>
-      <c r="D132" s="31">
+      <c r="A132" s="34"/>
+      <c r="B132" s="34"/>
+      <c r="C132" s="32"/>
+      <c r="D132" s="34">
         <v>4</v>
       </c>
-      <c r="E132" s="29" t="s">
+      <c r="E132" s="32" t="s">
         <v>156</v>
       </c>
       <c r="F132" s="4">
@@ -7721,158 +7723,158 @@
       <c r="G132" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="H132" s="30"/>
-      <c r="I132" s="31"/>
+      <c r="H132" s="31"/>
+      <c r="I132" s="34"/>
     </row>
     <row r="133" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A133" s="31"/>
-      <c r="B133" s="31"/>
-      <c r="C133" s="29"/>
-      <c r="D133" s="31"/>
-      <c r="E133" s="29"/>
+      <c r="A133" s="34"/>
+      <c r="B133" s="34"/>
+      <c r="C133" s="32"/>
+      <c r="D133" s="34"/>
+      <c r="E133" s="32"/>
       <c r="F133" s="4">
         <v>2</v>
       </c>
       <c r="G133" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="H133" s="30"/>
-      <c r="I133" s="31"/>
+      <c r="H133" s="31"/>
+      <c r="I133" s="34"/>
     </row>
     <row r="134" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A134" s="31"/>
-      <c r="B134" s="31"/>
-      <c r="C134" s="29"/>
-      <c r="D134" s="31"/>
-      <c r="E134" s="29"/>
+      <c r="A134" s="34"/>
+      <c r="B134" s="34"/>
+      <c r="C134" s="32"/>
+      <c r="D134" s="34"/>
+      <c r="E134" s="32"/>
       <c r="F134" s="4">
         <v>3</v>
       </c>
       <c r="G134" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="H134" s="30"/>
-      <c r="I134" s="31"/>
+      <c r="H134" s="31"/>
+      <c r="I134" s="34"/>
     </row>
     <row r="135" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A135" s="31"/>
-      <c r="B135" s="31"/>
-      <c r="C135" s="29"/>
-      <c r="D135" s="31"/>
-      <c r="E135" s="29"/>
+      <c r="A135" s="34"/>
+      <c r="B135" s="34"/>
+      <c r="C135" s="32"/>
+      <c r="D135" s="34"/>
+      <c r="E135" s="32"/>
       <c r="F135" s="4">
         <v>4</v>
       </c>
       <c r="G135" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="H135" s="30"/>
-      <c r="I135" s="31"/>
+      <c r="H135" s="31"/>
+      <c r="I135" s="34"/>
     </row>
     <row r="136" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A136" s="31"/>
-      <c r="B136" s="31"/>
-      <c r="C136" s="29"/>
-      <c r="D136" s="31"/>
-      <c r="E136" s="29"/>
+      <c r="A136" s="34"/>
+      <c r="B136" s="34"/>
+      <c r="C136" s="32"/>
+      <c r="D136" s="34"/>
+      <c r="E136" s="32"/>
       <c r="F136" s="4">
         <v>5</v>
       </c>
       <c r="G136" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="H136" s="30"/>
-      <c r="I136" s="31"/>
+      <c r="H136" s="31"/>
+      <c r="I136" s="34"/>
     </row>
     <row r="137" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A137" s="31"/>
-      <c r="B137" s="31"/>
-      <c r="C137" s="29"/>
-      <c r="D137" s="31"/>
-      <c r="E137" s="29"/>
+      <c r="A137" s="34"/>
+      <c r="B137" s="34"/>
+      <c r="C137" s="32"/>
+      <c r="D137" s="34"/>
+      <c r="E137" s="32"/>
       <c r="F137" s="4">
         <v>6</v>
       </c>
       <c r="G137" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="H137" s="30"/>
-      <c r="I137" s="31"/>
+      <c r="H137" s="31"/>
+      <c r="I137" s="34"/>
     </row>
     <row r="138" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A138" s="31"/>
-      <c r="B138" s="31"/>
-      <c r="C138" s="29"/>
-      <c r="D138" s="31"/>
-      <c r="E138" s="29"/>
+      <c r="A138" s="34"/>
+      <c r="B138" s="34"/>
+      <c r="C138" s="32"/>
+      <c r="D138" s="34"/>
+      <c r="E138" s="32"/>
       <c r="F138" s="4">
         <v>7</v>
       </c>
       <c r="G138" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="H138" s="30"/>
-      <c r="I138" s="31"/>
+      <c r="H138" s="31"/>
+      <c r="I138" s="34"/>
     </row>
     <row r="139" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A139" s="31"/>
-      <c r="B139" s="31"/>
-      <c r="C139" s="29"/>
-      <c r="D139" s="31"/>
-      <c r="E139" s="29"/>
+      <c r="A139" s="34"/>
+      <c r="B139" s="34"/>
+      <c r="C139" s="32"/>
+      <c r="D139" s="34"/>
+      <c r="E139" s="32"/>
       <c r="F139" s="4">
         <v>8</v>
       </c>
       <c r="G139" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="H139" s="30"/>
-      <c r="I139" s="31"/>
+      <c r="H139" s="31"/>
+      <c r="I139" s="34"/>
     </row>
     <row r="140" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A140" s="31"/>
-      <c r="B140" s="31"/>
-      <c r="C140" s="29"/>
-      <c r="D140" s="31"/>
-      <c r="E140" s="29"/>
+      <c r="A140" s="34"/>
+      <c r="B140" s="34"/>
+      <c r="C140" s="32"/>
+      <c r="D140" s="34"/>
+      <c r="E140" s="32"/>
       <c r="F140" s="4">
         <v>9</v>
       </c>
       <c r="G140" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="H140" s="30"/>
-      <c r="I140" s="31"/>
+      <c r="H140" s="31"/>
+      <c r="I140" s="34"/>
     </row>
     <row r="141" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A141" s="31"/>
-      <c r="B141" s="31"/>
-      <c r="C141" s="29"/>
-      <c r="D141" s="31"/>
-      <c r="E141" s="29"/>
+      <c r="A141" s="34"/>
+      <c r="B141" s="34"/>
+      <c r="C141" s="32"/>
+      <c r="D141" s="34"/>
+      <c r="E141" s="32"/>
       <c r="F141" s="4">
         <v>10</v>
       </c>
       <c r="G141" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="H141" s="30"/>
-      <c r="I141" s="31"/>
+      <c r="H141" s="31"/>
+      <c r="I141" s="34"/>
     </row>
     <row r="142" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A142" s="31"/>
-      <c r="B142" s="31"/>
-      <c r="C142" s="29"/>
-      <c r="D142" s="31"/>
-      <c r="E142" s="29"/>
+      <c r="A142" s="34"/>
+      <c r="B142" s="34"/>
+      <c r="C142" s="32"/>
+      <c r="D142" s="34"/>
+      <c r="E142" s="32"/>
       <c r="F142" s="4">
         <v>11</v>
       </c>
       <c r="G142" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="H142" s="30"/>
-      <c r="I142" s="31"/>
+      <c r="H142" s="31"/>
+      <c r="I142" s="34"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
@@ -7886,48 +7888,69 @@
       <c r="I143" s="4"/>
     </row>
     <row r="144" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A144" s="32" t="s">
+      <c r="A144" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="B144" s="32"/>
-      <c r="C144" s="32" t="s">
+      <c r="B144" s="36"/>
+      <c r="C144" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D144" s="32"/>
-      <c r="E144" s="32"/>
-      <c r="F144" s="32"/>
-      <c r="G144" s="32"/>
+      <c r="D144" s="36"/>
+      <c r="E144" s="36"/>
+      <c r="F144" s="36"/>
+      <c r="G144" s="36"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
     </row>
     <row r="145" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A145" s="32" t="s">
+      <c r="A145" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="B145" s="32"/>
-      <c r="C145" s="32"/>
-      <c r="D145" s="32"/>
-      <c r="E145" s="32"/>
-      <c r="F145" s="32"/>
-      <c r="G145" s="32"/>
+      <c r="B145" s="36"/>
+      <c r="C145" s="36"/>
+      <c r="D145" s="36"/>
+      <c r="E145" s="36"/>
+      <c r="F145" s="36"/>
+      <c r="G145" s="36"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="E2:E15"/>
-    <mergeCell ref="E16:E21"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="E27:E33"/>
-    <mergeCell ref="C35:C74"/>
-    <mergeCell ref="E35:E44"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="E58:E63"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="D35:D44"/>
-    <mergeCell ref="C2:C33"/>
-    <mergeCell ref="E53:E57"/>
+    <mergeCell ref="H111:H142"/>
+    <mergeCell ref="I111:I142"/>
+    <mergeCell ref="H2:H33"/>
+    <mergeCell ref="I2:I33"/>
+    <mergeCell ref="H35:H74"/>
+    <mergeCell ref="I35:I74"/>
+    <mergeCell ref="H76:H109"/>
+    <mergeCell ref="I76:I109"/>
+    <mergeCell ref="E105:E109"/>
+    <mergeCell ref="D95:D104"/>
+    <mergeCell ref="D105:D109"/>
+    <mergeCell ref="D111:D114"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E76:E82"/>
+    <mergeCell ref="E83:E85"/>
+    <mergeCell ref="E86:E91"/>
+    <mergeCell ref="E92:E94"/>
+    <mergeCell ref="E95:E104"/>
+    <mergeCell ref="B35:B74"/>
+    <mergeCell ref="B76:B109"/>
+    <mergeCell ref="B111:B142"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="D53:D57"/>
+    <mergeCell ref="D58:D63"/>
+    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="D132:D142"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D76:D82"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="D86:D91"/>
+    <mergeCell ref="D92:D94"/>
+    <mergeCell ref="D118:D131"/>
     <mergeCell ref="A144:B144"/>
     <mergeCell ref="C144:G144"/>
     <mergeCell ref="A145:G145"/>
@@ -7944,40 +7967,19 @@
     <mergeCell ref="E64:E68"/>
     <mergeCell ref="E69:E71"/>
     <mergeCell ref="C76:C109"/>
-    <mergeCell ref="B35:B74"/>
-    <mergeCell ref="B76:B109"/>
-    <mergeCell ref="B111:B142"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="D58:D63"/>
-    <mergeCell ref="D64:D68"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="D132:D142"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D76:D82"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="D86:D91"/>
-    <mergeCell ref="D92:D94"/>
-    <mergeCell ref="D118:D131"/>
-    <mergeCell ref="E76:E82"/>
-    <mergeCell ref="E83:E85"/>
-    <mergeCell ref="E86:E91"/>
-    <mergeCell ref="E92:E94"/>
-    <mergeCell ref="E95:E104"/>
-    <mergeCell ref="E105:E109"/>
-    <mergeCell ref="D95:D104"/>
-    <mergeCell ref="D105:D109"/>
-    <mergeCell ref="D111:D114"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="H111:H142"/>
-    <mergeCell ref="I111:I142"/>
-    <mergeCell ref="H2:H33"/>
-    <mergeCell ref="I2:I33"/>
-    <mergeCell ref="H35:H74"/>
-    <mergeCell ref="I35:I74"/>
-    <mergeCell ref="H76:H109"/>
-    <mergeCell ref="I76:I109"/>
+    <mergeCell ref="E2:E15"/>
+    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="C35:C74"/>
+    <mergeCell ref="E35:E44"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="E58:E63"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="D35:D44"/>
+    <mergeCell ref="C2:C33"/>
+    <mergeCell ref="E53:E57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8001,274 +8003,274 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="28" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="29" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="29" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="29" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="29" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="29" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="29" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="29" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="66" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="29" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="29" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="29" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="29" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="29" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="29" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>